<commit_message>
conclusion and future work
</commit_message>
<xml_diff>
--- a/project_yelp_recommendation/tables_4_presentation.xlsx
+++ b/project_yelp_recommendation/tables_4_presentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SOEN_499 Project\yelp-data-analysis\project_yelp_recommendation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F51E2AD-B76D-4FBE-A0C9-3F4759241CB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38819CCB-4599-4A7A-ADD6-01951FC12E33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4176" yWindow="456" windowWidth="28044" windowHeight="16584" xr2:uid="{17D7A015-5916-8846-B6E5-58D3E7395B48}"/>
+    <workbookView xWindow="5124" yWindow="456" windowWidth="28044" windowHeight="16584" xr2:uid="{17D7A015-5916-8846-B6E5-58D3E7395B48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Dataset introduction</t>
   </si>
@@ -168,6 +168,21 @@
   </si>
   <si>
     <t>5. Wu0yySWcHQ5tZ_59HNiamg</t>
+  </si>
+  <si>
+    <t>1. M8X 1E9</t>
+  </si>
+  <si>
+    <t>2. M5A 2L2</t>
+  </si>
+  <si>
+    <t>3. M6K 1L4</t>
+  </si>
+  <si>
+    <t>4. 89109</t>
+  </si>
+  <si>
+    <t>5. M6K</t>
   </si>
 </sst>
 </file>
@@ -549,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291F1A05-E2B6-9741-AF08-E9AB101E6CC1}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -744,7 +759,10 @@
         <v>1.7221782768440601</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
       <c r="F17" t="s">
         <v>26</v>
       </c>
@@ -752,7 +770,7 @@
         <v>1.2425122982974599</v>
       </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
         <v>27</v>
       </c>
@@ -760,12 +778,20 @@
         <v>2.55470156320228</v>
       </c>
     </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
       <c r="F21" t="s">
         <v>16</v>
       </c>
@@ -773,7 +799,7 @@
         <v>2.1478470949668198</v>
       </c>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
         <v>17</v>
       </c>
@@ -781,7 +807,10 @@
         <v>1.4353005646714201</v>
       </c>
     </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
       <c r="F23" t="s">
         <v>18</v>
       </c>
@@ -789,7 +818,10 @@
         <v>3.02685856977986</v>
       </c>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
       <c r="F25" t="s">
         <v>25</v>
       </c>
@@ -797,7 +829,7 @@
         <v>1.7175697991586001</v>
       </c>
     </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
         <v>26</v>
       </c>
@@ -805,7 +837,7 @@
         <v>1.2425122982974599</v>
       </c>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
         <v>27</v>
       </c>
@@ -813,12 +845,12 @@
         <v>2.5896254470859699</v>
       </c>
     </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F29" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
         <v>16</v>
       </c>
@@ -826,7 +858,7 @@
         <v>1.85259797843684</v>
       </c>
     </row>
-    <row r="31" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
         <v>17</v>
       </c>
@@ -834,7 +866,7 @@
         <v>1.3290577867732001</v>
       </c>
     </row>
-    <row r="32" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
         <v>18</v>
       </c>

</xml_diff>